<commit_message>
Add --checker flag for detailed integrity reports and update documentation
</commit_message>
<xml_diff>
--- a/tests/Full_Accounting_Test_Case.xlsx
+++ b/tests/Full_Accounting_Test_Case.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="62">
   <si>
     <t>Category</t>
   </si>
@@ -62,6 +62,9 @@
     <t>P&amp;L</t>
   </si>
   <si>
+    <t>Starbucks</t>
+  </si>
+  <si>
     <t>Bank Transactions</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
     <t>Expense</t>
   </si>
   <si>
+    <t>Amazon</t>
+  </si>
+  <si>
     <t>Credit Card Transactions</t>
   </si>
   <si>
@@ -96,6 +102,9 @@
   </si>
   <si>
     <t>Balance Sheet</t>
+  </si>
+  <si>
+    <t>AWS</t>
   </si>
   <si>
     <t>Credit Card</t>
@@ -164,6 +173,18 @@
     <t>Consulting Services</t>
   </si>
   <si>
+    <t>Mystery Corp</t>
+  </si>
+  <si>
+    <t>IllegalCat</t>
+  </si>
+  <si>
+    <t>UnknownVendor</t>
+  </si>
+  <si>
+    <t>Uncategorized Expense</t>
+  </si>
+  <si>
     <t>Member</t>
   </si>
   <si>
@@ -173,19 +194,10 @@
     <t>Receipt</t>
   </si>
   <si>
-    <t>Starbucks</t>
-  </si>
-  <si>
     <t>Coffee</t>
   </si>
   <si>
-    <t>Amazon</t>
-  </si>
-  <si>
     <t>Office Supplies</t>
-  </si>
-  <si>
-    <t>AWS</t>
   </si>
   <si>
     <t>Cloud Services</t>
@@ -631,14 +643,17 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -646,81 +661,87 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -728,13 +749,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -748,7 +769,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I500"/>
+  <dimension ref="A1:I502"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
@@ -762,13 +783,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -777,16 +798,16 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -794,7 +815,7 @@
         <v>45658</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>5000</v>
@@ -806,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -823,19 +844,19 @@
         <v>45662</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>-1500</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -852,7 +873,7 @@
         <v>45667</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>2500</v>
@@ -864,7 +885,7 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -3354,6 +3375,58 @@
     <row r="500" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I500">
         <f>IFERROR(VLOOKUP(D500,Setup!A:D,4,FALSE), "")</f>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A501" s="1">
+        <v>45682</v>
+      </c>
+      <c r="B501" t="s">
+        <v>52</v>
+      </c>
+      <c r="C501">
+        <v>100</v>
+      </c>
+      <c r="D501" t="s">
+        <v>53</v>
+      </c>
+      <c r="E501" t="s">
+        <v>4</v>
+      </c>
+      <c r="F501" t="s">
+        <v>4</v>
+      </c>
+      <c r="G501" t="s">
+        <v>54</v>
+      </c>
+      <c r="H501" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A502" s="1">
+        <v>45683</v>
+      </c>
+      <c r="B502" t="s">
+        <v>55</v>
+      </c>
+      <c r="C502">
+        <v>50</v>
+      </c>
+      <c r="D502" t="s">
+        <v>4</v>
+      </c>
+      <c r="E502" t="s">
+        <v>4</v>
+      </c>
+      <c r="F502" t="s">
+        <v>4</v>
+      </c>
+      <c r="G502" t="s">
+        <v>4</v>
+      </c>
+      <c r="H502" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3408,16 +3481,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -3426,22 +3499,22 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="L1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3452,19 +3525,19 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>15.5</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -3490,19 +3563,19 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
@@ -3528,19 +3601,19 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -6084,22 +6157,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6107,10 +6180,10 @@
         <v>45658</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>1000</v>
@@ -6124,10 +6197,10 @@
         <v>45677</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>50</v>

</xml_diff>

<commit_message>
Fix Excel corruption by aligning history logs with 2-column VERSION tab layout
</commit_message>
<xml_diff>
--- a/tests/Full_Accounting_Test_Case.xlsx
+++ b/tests/Full_Accounting_Test_Case.xlsx
@@ -7,15 +7,16 @@
     <sheet sheetId="1" name="Setup" state="visible" r:id="rId4"/>
     <sheet sheetId="4" name="Ledger" state="visible" r:id="rId5"/>
     <sheet sheetId="5" name="Summary" state="visible" r:id="rId6"/>
-    <sheet sheetId="2" name="Bank Transactions" state="visible" r:id="rId7"/>
-    <sheet sheetId="3" name="Credit Card Transactions" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="VERSION" state="visible" r:id="rId7"/>
+    <sheet sheetId="2" name="Bank Transactions" state="visible" r:id="rId8"/>
+    <sheet sheetId="3" name="Credit Card Transactions" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
   <si>
     <t>Category</t>
   </si>
@@ -138,6 +139,46 @@
   </si>
   <si>
     <t>Audit Adjustment</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Version ID</t>
+  </si>
+  <si>
+    <t>1.0.0-java</t>
+  </si>
+  <si>
+    <t>Git SHA</t>
+  </si>
+  <si>
+    <t>86304a3ad5ac79ddcc38f25d89f4326fbcfd15b8</t>
+  </si>
+  <si>
+    <t>Generated At</t>
+  </si>
+  <si>
+    <t>12/22/2025, 10:43:42 AM</t>
+  </si>
+  <si>
+    <t>--- Import History ---</t>
+  </si>
+  <si>
+    <t>Import at 12/22/2025, 10:43:43 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Command: node load_transactions.js tests/example_bank.csv bank Test_Accounting.xlsx --clear
+Input: tests/example_bank.csv
+Target Sheet: Bank Transactions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Command: node load_transactions.js tests/example_cc.csv cc Test_Accounting.xlsx --clear
+Input: tests/example_cc.csv
+Target Sheet: Credit Card Transactions</t>
   </si>
   <si>
     <t>Amount</t>
@@ -236,9 +277,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,7 +833,7 @@
         <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -798,16 +842,16 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -815,7 +859,7 @@
         <v>45658</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C2">
         <v>5000</v>
@@ -827,7 +871,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -844,7 +888,7 @@
         <v>45662</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>-1500</v>
@@ -856,7 +900,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -873,7 +917,7 @@
         <v>45667</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C4">
         <v>2500</v>
@@ -885,7 +929,7 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -3382,13 +3426,13 @@
         <v>45682</v>
       </c>
       <c r="B501" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C501">
         <v>100</v>
       </c>
       <c r="D501" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E501" t="s">
         <v>4</v>
@@ -3397,7 +3441,7 @@
         <v>4</v>
       </c>
       <c r="G501" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="H501" t="s">
         <v>4</v>
@@ -3408,7 +3452,7 @@
         <v>45683</v>
       </c>
       <c r="B502" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C502">
         <v>50</v>
@@ -3484,13 +3528,13 @@
         <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -3499,22 +3543,22 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3537,7 +3581,7 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -3575,7 +3619,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
@@ -3613,7 +3657,7 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -6223,4 +6267,75 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Stop worksheet deletion to prevent Excel Table/Autofilter corruption
</commit_message>
<xml_diff>
--- a/tests/Full_Accounting_Test_Case.xlsx
+++ b/tests/Full_Accounting_Test_Case.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Setup" state="visible" r:id="rId4"/>
-    <sheet sheetId="4" name="Ledger" state="visible" r:id="rId5"/>
-    <sheet sheetId="5" name="Summary" state="visible" r:id="rId6"/>
-    <sheet sheetId="6" name="VERSION" state="visible" r:id="rId7"/>
-    <sheet sheetId="2" name="Bank Transactions" state="visible" r:id="rId8"/>
-    <sheet sheetId="3" name="Credit Card Transactions" state="visible" r:id="rId9"/>
+    <sheet sheetId="2" name="Bank Transactions" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Credit Card Transactions" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Ledger" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Summary" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="VERSION" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
   <si>
     <t>Category</t>
   </si>
@@ -126,6 +126,69 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Extended Details</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Report Type (Auto)</t>
+  </si>
+  <si>
+    <t>Salary Deposit</t>
+  </si>
+  <si>
+    <t>January Paycheck</t>
+  </si>
+  <si>
+    <t>Office Rent</t>
+  </si>
+  <si>
+    <t>Monthly Rent</t>
+  </si>
+  <si>
+    <t>Client A Payment</t>
+  </si>
+  <si>
+    <t>Consulting Services</t>
+  </si>
+  <si>
+    <t>Mystery Corp</t>
+  </si>
+  <si>
+    <t>IllegalCat</t>
+  </si>
+  <si>
+    <t>UnknownVendor</t>
+  </si>
+  <si>
+    <t>Uncategorized Expense</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Account #</t>
+  </si>
+  <si>
+    <t>Receipt</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Office Supplies</t>
+  </si>
+  <si>
+    <t>Cloud Services</t>
+  </si>
+  <si>
     <t>Debit</t>
   </si>
   <si>
@@ -156,19 +219,19 @@
     <t>Git SHA</t>
   </si>
   <si>
-    <t>86304a3ad5ac79ddcc38f25d89f4326fbcfd15b8</t>
+    <t>73e7d18d43b5c9cddc6ec897fff356a5ef31c615</t>
   </si>
   <si>
     <t>Generated At</t>
   </si>
   <si>
-    <t>12/22/2025, 10:43:42 AM</t>
+    <t>12/22/2025, 10:47:42 AM</t>
   </si>
   <si>
     <t>--- Import History ---</t>
   </si>
   <si>
-    <t>Import at 12/22/2025, 10:43:43 AM</t>
+    <t>Import at 12/22/2025, 10:47:42 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Command: node load_transactions.js tests/example_bank.csv bank Test_Accounting.xlsx --clear
@@ -176,72 +239,12 @@
 Target Sheet: Bank Transactions</t>
   </si>
   <si>
+    <t>Import at 12/22/2025, 10:47:43 AM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Command: node load_transactions.js tests/example_cc.csv cc Test_Accounting.xlsx --clear
 Input: tests/example_cc.csv
 Target Sheet: Credit Card Transactions</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Extended Details</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Report Type (Auto)</t>
-  </si>
-  <si>
-    <t>Salary Deposit</t>
-  </si>
-  <si>
-    <t>January Paycheck</t>
-  </si>
-  <si>
-    <t>Office Rent</t>
-  </si>
-  <si>
-    <t>Monthly Rent</t>
-  </si>
-  <si>
-    <t>Client A Payment</t>
-  </si>
-  <si>
-    <t>Consulting Services</t>
-  </si>
-  <si>
-    <t>Mystery Corp</t>
-  </si>
-  <si>
-    <t>IllegalCat</t>
-  </si>
-  <si>
-    <t>UnknownVendor</t>
-  </si>
-  <si>
-    <t>Uncategorized Expense</t>
-  </si>
-  <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>Account #</t>
-  </si>
-  <si>
-    <t>Receipt</t>
-  </si>
-  <si>
-    <t>Coffee</t>
-  </si>
-  <si>
-    <t>Office Supplies</t>
-  </si>
-  <si>
-    <t>Cloud Services</t>
   </si>
 </sst>
 </file>
@@ -833,7 +836,7 @@
         <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -842,16 +845,16 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -859,7 +862,7 @@
         <v>45658</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>5000</v>
@@ -871,7 +874,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -888,7 +891,7 @@
         <v>45662</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>-1500</v>
@@ -900,7 +903,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -917,7 +920,7 @@
         <v>45667</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>2500</v>
@@ -929,7 +932,7 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -3426,13 +3429,13 @@
         <v>45682</v>
       </c>
       <c r="B501" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C501">
         <v>100</v>
       </c>
       <c r="D501" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E501" t="s">
         <v>4</v>
@@ -3441,7 +3444,7 @@
         <v>4</v>
       </c>
       <c r="G501" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="H501" t="s">
         <v>4</v>
@@ -3452,7 +3455,7 @@
         <v>45683</v>
       </c>
       <c r="B502" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C502">
         <v>50</v>
@@ -3528,13 +3531,13 @@
         <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -3543,22 +3546,22 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="K1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="L1" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3581,7 +3584,7 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -3619,7 +3622,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
@@ -3657,7 +3660,7 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -6210,13 +6213,13 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6224,7 +6227,7 @@
         <v>45658</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -6241,7 +6244,7 @@
         <v>45677</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -6280,39 +6283,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -6320,18 +6323,18 @@
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eliminate Excel Table corruption by removing redundant column definitions and autofilter conflicts
</commit_message>
<xml_diff>
--- a/tests/Full_Accounting_Test_Case.xlsx
+++ b/tests/Full_Accounting_Test_Case.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
   <si>
     <t>Category</t>
   </si>
@@ -129,7 +129,7 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Extended Details</t>
+    <t>Extended</t>
   </si>
   <si>
     <t>Vendor</t>
@@ -138,7 +138,7 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>Report Type (Auto)</t>
+    <t>Type (Auto)</t>
   </si>
   <si>
     <t>Salary Deposit</t>
@@ -174,7 +174,7 @@
     <t>Member</t>
   </si>
   <si>
-    <t>Account #</t>
+    <t>Acct #</t>
   </si>
   <si>
     <t>Receipt</t>
@@ -195,9 +195,6 @@
     <t>Credit</t>
   </si>
   <si>
-    <t>Type (Auto)</t>
-  </si>
-  <si>
     <t>Owner Investment</t>
   </si>
   <si>
@@ -219,19 +216,19 @@
     <t>Git SHA</t>
   </si>
   <si>
-    <t>73e7d18d43b5c9cddc6ec897fff356a5ef31c615</t>
+    <t>e1bc9b5f61053e9097c9a7b126b4faf92d218354</t>
   </si>
   <si>
     <t>Generated At</t>
   </si>
   <si>
-    <t>12/22/2025, 10:47:42 AM</t>
+    <t>12/22/2025, 10:51:21 AM</t>
   </si>
   <si>
     <t>--- Import History ---</t>
   </si>
   <si>
-    <t>Import at 12/22/2025, 10:47:42 AM</t>
+    <t>Import at 12/22/2025, 10:51:21 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Command: node load_transactions.js tests/example_bank.csv bank Test_Accounting.xlsx --clear
@@ -239,7 +236,7 @@
 Target Sheet: Bank Transactions</t>
   </si>
   <si>
-    <t>Import at 12/22/2025, 10:47:43 AM</t>
+    <t>Import at 12/22/2025, 10:51:22 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Command: node load_transactions.js tests/example_cc.csv cc Test_Accounting.xlsx --clear
@@ -3477,7 +3474,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" sqref="D10:D500">
       <formula1>Setup!$A$2:$A$100</formula1>
@@ -6159,7 +6155,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1"/>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" sqref="E10:E500">
       <formula1>Setup!$A$2:$A$100</formula1>
@@ -6219,7 +6214,7 @@
         <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6227,7 +6222,7 @@
         <v>45658</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -6244,7 +6239,7 @@
         <v>45677</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -6283,39 +6278,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
         <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -6323,18 +6318,18 @@
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Robust column mapping, Ledger integration fix, and Balance Sheet reporting update (v1.1.0)
</commit_message>
<xml_diff>
--- a/tests/Full_Accounting_Test_Case.xlsx
+++ b/tests/Full_Accounting_Test_Case.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Setup" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Bank Transactions" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Credit Card Transactions" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Ledger" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="Summary" state="visible" r:id="rId8"/>
-    <sheet sheetId="6" name="VERSION" state="visible" r:id="rId9"/>
+    <sheet sheetId="4" name="Ledger" state="visible" r:id="rId5"/>
+    <sheet sheetId="5" name="Summary" state="visible" r:id="rId6"/>
+    <sheet sheetId="6" name="VERSION" state="visible" r:id="rId7"/>
+    <sheet sheetId="2" name="Bank Transactions" state="visible" r:id="rId8"/>
+    <sheet sheetId="3" name="Credit Card Transactions" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -120,81 +120,12 @@
     <t>Travel</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>SUBTOTAL (Filtered)</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Extended Details</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Report Type (Auto)</t>
-  </si>
-  <si>
-    <t>Salary Deposit</t>
-  </si>
-  <si>
-    <t>January Paycheck</t>
-  </si>
-  <si>
-    <t>Office Rent</t>
-  </si>
-  <si>
-    <t>Monthly Rent</t>
-  </si>
-  <si>
-    <t>Client A Payment</t>
-  </si>
-  <si>
-    <t>Consulting Services</t>
-  </si>
-  <si>
-    <t>Mystery Corp</t>
-  </si>
-  <si>
-    <t>IllegalCat</t>
-  </si>
-  <si>
-    <t>UnknownVendor</t>
-  </si>
-  <si>
-    <t>Uncategorized Expense</t>
-  </si>
-  <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>Account #</t>
-  </si>
-  <si>
-    <t>Receipt</t>
-  </si>
-  <si>
-    <t>Coffee</t>
-  </si>
-  <si>
-    <t>Office Supplies</t>
-  </si>
-  <si>
-    <t>Cloud Services</t>
-  </si>
-  <si>
     <t>Debit</t>
   </si>
   <si>
@@ -225,19 +156,19 @@
     <t>Git SHA</t>
   </si>
   <si>
-    <t>c4e56fe013a6d94cd8883059d43cd522c84d40de</t>
+    <t>26ac5083a346b8249d74ad044b15a439caad22cf</t>
   </si>
   <si>
     <t>Generated At</t>
   </si>
   <si>
-    <t>12/22/2025, 11:58:38 AM</t>
+    <t>12/26/2025, 9:05:48 PM</t>
   </si>
   <si>
     <t>--- Import History ---</t>
   </si>
   <si>
-    <t>Import at 12/22/2025, 11:58:39 AM</t>
+    <t>Import at 12/26/2025, 9:05:49 PM</t>
   </si>
   <si>
     <t xml:space="preserve">Command: node load_transactions.js tests/example_bank.csv bank Test_Accounting.xlsx --clear
@@ -248,13 +179,82 @@
     <t xml:space="preserve">Command: node load_transactions.js tests/example_cc.csv cc Test_Accounting.xlsx --clear
 Input: tests/example_cc.csv
 Target Sheet: Credit Card Transactions</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>SUBTOTAL (Filtered)</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Extended Details</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Report Type (Auto)</t>
+  </si>
+  <si>
+    <t>Salary Deposit</t>
+  </si>
+  <si>
+    <t>January Paycheck</t>
+  </si>
+  <si>
+    <t>Office Rent</t>
+  </si>
+  <si>
+    <t>Monthly Rent</t>
+  </si>
+  <si>
+    <t>Client A Payment</t>
+  </si>
+  <si>
+    <t>Consulting Services</t>
+  </si>
+  <si>
+    <t>Mystery Corp</t>
+  </si>
+  <si>
+    <t>IllegalCat</t>
+  </si>
+  <si>
+    <t>UnknownVendor</t>
+  </si>
+  <si>
+    <t>Uncategorized Expense</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>Receipt</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Office Supplies</t>
+  </si>
+  <si>
+    <t>Cloud Services</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -269,13 +269,22 @@
       <b/>
       <i/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4F81BD"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -290,14 +299,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -313,68 +323,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="Table_BankTransactions_1766433519319" displayName="Table_BankTransactions_1766433519319" ref="A3:I6" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A3:I6">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Description" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Amount" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Category" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Sub-Category" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Extended Details" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Vendor" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Customer" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Report Type (Auto)" totalsRowFunction="none"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" name="Table_CreditCardTransactions_1766433519706" displayName="Table_CreditCardTransactions_1766433519706" ref="A3:L6" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A3:L6">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-    <filterColumn colId="11" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="12">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Member" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Description" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Amount" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Category" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Sub-Category" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Extended Details" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Vendor" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Customer" totalsRowFunction="none"/>
-    <tableColumn id="10" name="Account #" totalsRowFunction="none"/>
-    <tableColumn id="11" name="Receipt" totalsRowFunction="none"/>
-    <tableColumn id="12" name="Report Type (Auto)" totalsRowFunction="none"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -903,56 +851,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3">
+        <f>SUM(C4:C10000)</f>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="4">
+        <f>SUBTOTAL(109, C4:C10000)</f>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1">
-        <f>SUM(C4:C10000)</f>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="2">
-        <f>SUBTOTAL(109, C4:C10000)</f>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" t="s">
-        <v>42</v>
+      <c r="F3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>45658</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C4">
         <v>5000</v>
@@ -964,7 +912,7 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -977,11 +925,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>45662</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>-1500</v>
@@ -993,7 +941,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -1006,11 +954,11 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>45667</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C6">
         <v>2500</v>
@@ -1022,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -1035,17 +983,17 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>45682</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -1054,18 +1002,18 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>45683</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -1087,6 +1035,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:I6"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" sqref="D4:D6">
       <formula1>Setup!$A$2:$A$100</formula1>
@@ -1103,9 +1052,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -1120,68 +1066,67 @@
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="8" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="3">
+        <f>SUM(D4:D10000)</f>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="4">
+        <f>SUBTOTAL(109, D4:D10000)</f>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1">
-        <f>SUM(D4:D10000)</f>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="2">
-        <f>SUBTOTAL(109, D4:D10000)</f>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" t="s">
-        <v>42</v>
+      <c r="G3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>45659</v>
       </c>
       <c r="B4" t="s">
@@ -1200,7 +1145,7 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -1219,7 +1164,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>45663</v>
       </c>
       <c r="B5" t="s">
@@ -1238,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
@@ -1257,7 +1202,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>45669</v>
       </c>
       <c r="B6" t="s">
@@ -1276,7 +1221,7 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="H6" t="s">
         <v>4</v>
@@ -1295,6 +1240,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:L6"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" sqref="E4:E6">
       <formula1>Setup!$A$2:$A$100</formula1>
@@ -1311,9 +1257,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -1330,30 +1273,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>45658</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -1366,11 +1309,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>45677</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -1409,58 +1352,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>75</v>
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance Setup table decoupling and improve financial linkage logic
</commit_message>
<xml_diff>
--- a/tests/Full_Accounting_Test_Case.xlsx
+++ b/tests/Full_Accounting_Test_Case.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="77">
   <si>
     <t>Category</t>
   </si>
@@ -150,30 +150,33 @@
     <t>Version ID</t>
   </si>
   <si>
-    <t>1.0.0-java</t>
+    <t>1.1.0</t>
   </si>
   <si>
     <t>Git SHA</t>
   </si>
   <si>
-    <t>26ac5083a346b8249d74ad044b15a439caad22cf</t>
+    <t>d30caf8818b4bcec55d88484ee588c128f9dcf14</t>
   </si>
   <si>
     <t>Generated At</t>
   </si>
   <si>
-    <t>12/26/2025, 9:05:48 PM</t>
+    <t>12/30/2025, 11:11:02 AM</t>
   </si>
   <si>
     <t>--- Import History ---</t>
   </si>
   <si>
-    <t>Import at 12/26/2025, 9:05:49 PM</t>
+    <t>Import at 12/30/2025, 11:11:02 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Command: node load_transactions.js tests/example_bank.csv bank Test_Accounting.xlsx --clear
 Input: tests/example_bank.csv
 Target Sheet: Bank Transactions</t>
+  </si>
+  <si>
+    <t>Import at 12/30/2025, 11:11:03 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Command: node load_transactions.js tests/example_cc.csv cc Test_Accounting.xlsx --clear
@@ -779,7 +782,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -852,7 +855,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" s="3">
         <f>SUM(C4:C10000)</f>
@@ -860,7 +863,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C2" s="4">
         <f>SUBTOTAL(109, C4:C10000)</f>
@@ -874,7 +877,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>0</v>
@@ -883,16 +886,16 @@
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -900,7 +903,7 @@
         <v>45658</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>5000</v>
@@ -912,7 +915,7 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -929,7 +932,7 @@
         <v>45662</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>-1500</v>
@@ -941,7 +944,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -958,7 +961,7 @@
         <v>45667</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C6">
         <v>2500</v>
@@ -970,7 +973,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -987,13 +990,13 @@
         <v>45682</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -1002,7 +1005,7 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
@@ -1013,7 +1016,7 @@
         <v>45683</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -1073,7 +1076,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D1" s="3">
         <f>SUM(D4:D10000)</f>
@@ -1081,7 +1084,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" s="4">
         <f>SUBTOTAL(109, D4:D10000)</f>
@@ -1092,13 +1095,13 @@
         <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>0</v>
@@ -1107,22 +1110,22 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1145,7 +1148,7 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -1183,7 +1186,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
@@ -1221,7 +1224,7 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H6" t="s">
         <v>4</v>
@@ -1400,10 +1403,10 @@
     </row>
     <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>